<commit_message>
added ppt and results
</commit_message>
<xml_diff>
--- a/review_docs/results.xlsx
+++ b/review_docs/results.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nishant\Documents\thesis\thesis\review_docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30AB5681-72BE-4240-8364-9AF128D30A19}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A67BF33E-58E8-44B9-A72E-751B4B0DB58C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" activeTab="6" xr2:uid="{00DAEF19-75ED-4CFC-B6E9-28794BE537C5}"/>
   </bookViews>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="207" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="211" uniqueCount="18">
   <si>
     <t>first with one hot for all</t>
   </si>
@@ -95,18 +95,12 @@
   <si>
     <t>random guess log loss=0.33</t>
   </si>
-  <si>
-    <t>l</t>
-  </si>
-  <si>
-    <t>c</t>
-  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -121,17 +115,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="7"/>
-      <name val="Courier New"/>
-      <family val="3"/>
-    </font>
-    <font>
-      <sz val="7"/>
-      <color rgb="FF212121"/>
-      <name val="Courier New"/>
-      <family val="3"/>
     </font>
   </fonts>
   <fills count="2">
@@ -154,14 +137,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2724,7 +2705,7 @@
   <dimension ref="A1:E17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3:E17"/>
+      <selection activeCell="A21" sqref="A21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3548,7 +3529,7 @@
   <dimension ref="A1:H17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+      <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3587,8 +3568,17 @@
       <c r="A3" t="s">
         <v>3</v>
       </c>
+      <c r="B3">
+        <v>0.90653071133770302</v>
+      </c>
+      <c r="C3">
+        <v>0.91539208545763495</v>
+      </c>
       <c r="D3">
         <v>0.92024763292061096</v>
+      </c>
+      <c r="E3">
+        <v>0.91891235736829302</v>
       </c>
       <c r="H3" s="2"/>
     </row>
@@ -3596,8 +3586,17 @@
       <c r="A4" t="s">
         <v>4</v>
       </c>
+      <c r="B4">
+        <v>0.67756977992485201</v>
+      </c>
+      <c r="C4">
+        <v>0.77730364118878403</v>
+      </c>
       <c r="D4">
         <v>0.78923495710742397</v>
+      </c>
+      <c r="E4">
+        <v>0.777441577738754</v>
       </c>
       <c r="H4" s="2"/>
     </row>
@@ -3605,8 +3604,17 @@
       <c r="A5" t="s">
         <v>5</v>
       </c>
+      <c r="B5">
+        <v>0.19939769053700501</v>
+      </c>
+      <c r="C5">
+        <v>0.18272958949412099</v>
+      </c>
       <c r="D5">
         <v>0.17195301127343299</v>
+      </c>
+      <c r="E5">
+        <v>0.17493075043161599</v>
       </c>
       <c r="H5" s="2"/>
     </row>
@@ -3738,8 +3746,11 @@
       <c r="C15" t="s">
         <v>12</v>
       </c>
-      <c r="D15" s="4">
+      <c r="D15">
         <v>0.91988346686088796</v>
+      </c>
+      <c r="E15">
+        <v>0.91927652342801602</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.35">
@@ -3752,11 +3763,14 @@
       <c r="C16" t="s">
         <v>12</v>
       </c>
-      <c r="D16" s="4">
+      <c r="D16">
         <v>0.78965441467762698</v>
       </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E16">
+        <v>0.777375916455469</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>5</v>
       </c>
@@ -3766,13 +3780,316 @@
       <c r="C17" t="s">
         <v>12</v>
       </c>
-      <c r="D17" s="4">
+      <c r="D17">
         <v>0.17276499219864899</v>
       </c>
+      <c r="E17">
+        <v>0.177842210608117</v>
+      </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="B17:C17 E17">
-    <cfRule type="colorScale" priority="1">
+  <conditionalFormatting sqref="B15:C15">
+    <cfRule type="colorScale" priority="17">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B15:C15">
+    <cfRule type="colorScale" priority="16">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B16:C16">
+    <cfRule type="colorScale" priority="15">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B16:C16">
+    <cfRule type="colorScale" priority="14">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B17:C17">
+    <cfRule type="colorScale" priority="3">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B17:C17">
+    <cfRule type="colorScale" priority="2">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B11:C11">
+    <cfRule type="colorScale" priority="29">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B11:C11">
+    <cfRule type="colorScale" priority="28">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B12:C12">
+    <cfRule type="colorScale" priority="27">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B12:C12">
+    <cfRule type="colorScale" priority="26">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B11:E11">
+    <cfRule type="colorScale" priority="39">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B12:E12">
+    <cfRule type="colorScale" priority="40">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B7:C7">
+    <cfRule type="colorScale" priority="23">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B7:C7">
+    <cfRule type="colorScale" priority="22">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B8:C8">
+    <cfRule type="colorScale" priority="21">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B8:C8">
+    <cfRule type="colorScale" priority="20">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B7:E7">
+    <cfRule type="colorScale" priority="24">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B8:E8">
+    <cfRule type="colorScale" priority="25">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B9:C9">
+    <cfRule type="colorScale" priority="11">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B9:C9">
+    <cfRule type="colorScale" priority="10">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B9:E9">
+    <cfRule type="colorScale" priority="12">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B9:E9">
+    <cfRule type="colorScale" priority="9">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B13:C13">
+    <cfRule type="colorScale" priority="7">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B13:C13">
+    <cfRule type="colorScale" priority="6">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B13:E13">
+    <cfRule type="colorScale" priority="8">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B13:E13">
+    <cfRule type="colorScale" priority="5">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -3855,162 +4172,6 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B15:C15">
-    <cfRule type="colorScale" priority="17">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B15:C15">
-    <cfRule type="colorScale" priority="16">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B16:C16">
-    <cfRule type="colorScale" priority="15">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B16:C16">
-    <cfRule type="colorScale" priority="14">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B15:C15 E15">
-    <cfRule type="colorScale" priority="18">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B16:C16 E16">
-    <cfRule type="colorScale" priority="19">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B17:C17">
-    <cfRule type="colorScale" priority="3">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B17:C17">
-    <cfRule type="colorScale" priority="2">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B17:C17 E17">
-    <cfRule type="colorScale" priority="4">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FF63BE7B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FFF8696B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B11:C11">
-    <cfRule type="colorScale" priority="29">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B11:C11">
-    <cfRule type="colorScale" priority="28">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B12:C12">
-    <cfRule type="colorScale" priority="27">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B12:C12">
-    <cfRule type="colorScale" priority="26">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
   <conditionalFormatting sqref="B3:E3">
     <cfRule type="colorScale" priority="36">
       <colorScale>
@@ -4047,92 +4208,20 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B11:E11">
-    <cfRule type="colorScale" priority="39">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B12:E12">
-    <cfRule type="colorScale" priority="40">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B7:C7">
-    <cfRule type="colorScale" priority="23">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B7:C7">
-    <cfRule type="colorScale" priority="22">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B8:C8">
-    <cfRule type="colorScale" priority="21">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B8:C8">
-    <cfRule type="colorScale" priority="20">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B7:E7">
-    <cfRule type="colorScale" priority="24">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B8:E8">
-    <cfRule type="colorScale" priority="25">
+  <conditionalFormatting sqref="B15:E15">
+    <cfRule type="colorScale" priority="18">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B16:E16">
+    <cfRule type="colorScale" priority="19">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -4155,92 +4244,20 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B9:C9">
-    <cfRule type="colorScale" priority="11">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B9:C9">
-    <cfRule type="colorScale" priority="10">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B9:E9">
-    <cfRule type="colorScale" priority="12">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FF63BE7B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FFF8696B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B9:E9">
-    <cfRule type="colorScale" priority="9">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FF63BE7B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FFF8696B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B13:C13">
-    <cfRule type="colorScale" priority="7">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B13:C13">
-    <cfRule type="colorScale" priority="6">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B13:E13">
-    <cfRule type="colorScale" priority="8">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FF63BE7B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FFF8696B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B13:E13">
-    <cfRule type="colorScale" priority="5">
+  <conditionalFormatting sqref="B17:E17">
+    <cfRule type="colorScale" priority="4">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B17:E17">
+    <cfRule type="colorScale" priority="1">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -4258,10 +4275,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5DFF9A87-E2A5-4EFC-A17C-83CC320AA0AA}">
-  <dimension ref="A1:J17"/>
+  <dimension ref="A1:E17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I17" sqref="I17"/>
+      <selection activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -4269,7 +4286,7 @@
     <col min="1" max="1" width="23.81640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>10</v>
       </c>
@@ -4286,258 +4303,180 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>3</v>
       </c>
       <c r="B3">
-        <v>0.33333333333333298</v>
+        <v>0.35057471264367801</v>
       </c>
       <c r="C3">
-        <v>0.36206896551724099</v>
+        <v>0.35057471264367801</v>
       </c>
       <c r="D3">
-        <v>0.31034482758620602</v>
+        <v>0.32758620689655099</v>
       </c>
       <c r="E3">
         <v>0.356321839080459</v>
       </c>
-      <c r="G3" s="4">
-        <v>0.35057471264367801</v>
-      </c>
-      <c r="H3" s="4">
-        <v>0.35057471264367801</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>4</v>
       </c>
       <c r="B4">
-        <v>0.28711660102637498</v>
+        <v>0.31474718304791899</v>
       </c>
       <c r="C4">
-        <v>0.35907866753981899</v>
+        <v>0.34235175851717198</v>
       </c>
       <c r="D4">
-        <v>0.29846049375825501</v>
+        <v>0.31736249002047601</v>
       </c>
       <c r="E4">
-        <v>0.330317594879045</v>
-      </c>
-      <c r="G4" s="4">
-        <v>0.31474718304791899</v>
-      </c>
-      <c r="H4" s="4">
-        <v>0.34235175851717198</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
+        <v>0.33641619730329397</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>5</v>
       </c>
       <c r="B5">
-        <v>1.33238901478913</v>
+        <v>1.3147713078596901</v>
       </c>
       <c r="C5">
-        <v>1.64983242152301</v>
+        <v>1.6283606951360401</v>
       </c>
       <c r="D5">
-        <v>1.32271124311935</v>
+        <v>1.34328595739467</v>
       </c>
       <c r="E5">
-        <v>1.2946778170209099</v>
-      </c>
-      <c r="G5" s="4">
-        <v>1.3147713078596901</v>
-      </c>
-      <c r="H5" s="4">
-        <v>1.6283606951360401</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.35">
+        <v>1.29787621563677</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="I6" t="s">
-        <v>18</v>
-      </c>
-      <c r="J6" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.35">
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>3</v>
       </c>
       <c r="B7">
+        <v>0.31034482758620602</v>
+      </c>
+      <c r="C7">
+        <v>0.29310344827586199</v>
+      </c>
+      <c r="D7">
         <v>0.34482758620689602</v>
       </c>
-      <c r="C7">
-        <v>0.25287356321839</v>
-      </c>
-      <c r="D7">
-        <v>0.29310344827586199</v>
-      </c>
       <c r="E7">
-        <v>0.33333333333333298</v>
-      </c>
-      <c r="G7" s="4">
-        <v>0.31034482758620602</v>
-      </c>
-      <c r="H7" s="4">
-        <v>0.29310344827586199</v>
-      </c>
-      <c r="I7" s="3">
-        <v>0.34482758620689602</v>
-      </c>
-      <c r="J7" s="3">
         <v>0.32758620689655099</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>4</v>
       </c>
       <c r="B8">
-        <v>0.32508001988542601</v>
+        <v>0.29687001594896301</v>
       </c>
       <c r="C8">
-        <v>0.25199205901937399</v>
+        <v>0.29307608100711502</v>
       </c>
       <c r="D8">
-        <v>0.28598810410527098</v>
+        <v>0.346963955743259</v>
       </c>
       <c r="E8">
-        <v>0.32562851560857098</v>
-      </c>
-      <c r="G8" s="4">
-        <v>0.29687001594896301</v>
-      </c>
-      <c r="H8" s="4">
-        <v>0.29307608100711502</v>
-      </c>
-      <c r="I8" s="3">
-        <v>0.346963955743259</v>
-      </c>
-      <c r="J8" s="3">
         <v>0.32508288869859198</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>5</v>
       </c>
       <c r="B9">
-        <v>1.3411601894785301</v>
+        <v>1.33586638389416</v>
       </c>
       <c r="C9">
-        <v>2.6951273220849501</v>
+        <v>2.2273192973807401</v>
       </c>
       <c r="D9">
-        <v>1.43262041540745</v>
+        <v>1.3477724748417801</v>
       </c>
       <c r="E9">
-        <v>1.3653337707372</v>
-      </c>
-      <c r="G9" s="4">
-        <v>1.33586638389416</v>
-      </c>
-      <c r="H9" s="4">
-        <v>2.2273192973807401</v>
-      </c>
-      <c r="I9" s="3">
-        <v>1.3477724748417801</v>
-      </c>
-      <c r="J9" s="3">
         <v>1.35754336726876</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A10" s="1" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>3</v>
       </c>
       <c r="B11">
-        <v>0.31609195402298801</v>
+        <v>0.31034482758620602</v>
       </c>
       <c r="C11">
-        <v>0.26436781609195398</v>
+        <v>0.28735632183908</v>
       </c>
       <c r="D11">
         <v>0.31609195402298801</v>
       </c>
       <c r="E11">
-        <v>0.28735632183908</v>
-      </c>
-      <c r="G11" s="4">
-        <v>0.31034482758620602</v>
-      </c>
-      <c r="H11" s="4">
-        <v>0.28735632183908</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.35">
+        <v>0.29310344827586199</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>4</v>
       </c>
       <c r="B12">
-        <v>0.30191885964912202</v>
+        <v>0.29457115881534401</v>
       </c>
       <c r="C12">
-        <v>0.26468253968253902</v>
+        <v>0.28701594289021698</v>
       </c>
       <c r="D12">
-        <v>0.31115288949952002</v>
+        <v>0.317274810783649</v>
       </c>
       <c r="E12">
-        <v>0.28101790960998502</v>
-      </c>
-      <c r="G12" s="4">
-        <v>0.29457115881534401</v>
-      </c>
-      <c r="H12" s="4">
-        <v>0.28701594289021698</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.35">
+        <v>0.28683233385361001</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>5</v>
       </c>
       <c r="B13">
-        <v>1.3782878360448401</v>
+        <v>1.3477428731538701</v>
       </c>
       <c r="C13">
-        <v>2.2956347850876599</v>
+        <v>2.6384513016033901</v>
       </c>
       <c r="D13">
-        <v>1.3825469870493801</v>
+        <v>1.3848974521699799</v>
       </c>
       <c r="E13">
-        <v>1.3682507686779599</v>
-      </c>
-      <c r="G13" s="4">
-        <v>1.3477428731538701</v>
-      </c>
-      <c r="H13" s="4">
-        <v>2.6384513016033901</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.35">
+        <v>1.3611151519704501</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A14" s="1" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>3</v>
       </c>
@@ -4548,16 +4487,13 @@
         <v>12</v>
       </c>
       <c r="D15">
-        <v>0.34482758620689602</v>
+        <v>0.33908045977011397</v>
       </c>
       <c r="E15">
-        <v>0.35057471264367801</v>
-      </c>
-      <c r="I15" s="4">
-        <v>0.33908045977011397</v>
-      </c>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.35">
+        <v>0.36206896551724099</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>4</v>
       </c>
@@ -4568,16 +4504,13 @@
         <v>12</v>
       </c>
       <c r="D16">
-        <v>0.33896979729738802</v>
+        <v>0.33088772797584298</v>
       </c>
       <c r="E16">
-        <v>0.33692874590362898</v>
-      </c>
-      <c r="I16" s="4">
-        <v>0.33088772797584298</v>
-      </c>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.35">
+        <v>0.35488432456186803</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>5</v>
       </c>
@@ -4588,13 +4521,10 @@
         <v>12</v>
       </c>
       <c r="D17">
-        <v>1.69893963658081</v>
+        <v>1.3635438303960601</v>
       </c>
       <c r="E17">
-        <v>1.33323940742193</v>
-      </c>
-      <c r="I17" s="4">
-        <v>1.3635438303960601</v>
+        <v>1.34477519761917</v>
       </c>
     </row>
   </sheetData>
@@ -5088,7 +5018,7 @@
   <dimension ref="A1:E17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -5122,16 +5052,52 @@
       <c r="A3" t="s">
         <v>3</v>
       </c>
+      <c r="B3">
+        <v>0.78901734104046195</v>
+      </c>
+      <c r="C3">
+        <v>0.91329479768786104</v>
+      </c>
+      <c r="D3">
+        <v>0.78757225433526001</v>
+      </c>
+      <c r="E3">
+        <v>0.91184971098265899</v>
+      </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>4</v>
       </c>
+      <c r="B4">
+        <v>0.52252610461095095</v>
+      </c>
+      <c r="C4">
+        <v>0.704351049514784</v>
+      </c>
+      <c r="D4">
+        <v>0.48264971575491</v>
+      </c>
+      <c r="E4">
+        <v>0.68264648341938905</v>
+      </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>5</v>
       </c>
+      <c r="B5">
+        <v>0.71312473611139604</v>
+      </c>
+      <c r="C5">
+        <v>0.29762199704351899</v>
+      </c>
+      <c r="D5">
+        <v>0.58418482934854898</v>
+      </c>
+      <c r="E5">
+        <v>0.26896674392741199</v>
+      </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
@@ -5142,16 +5108,52 @@
       <c r="A7" t="s">
         <v>3</v>
       </c>
+      <c r="B7">
+        <v>0.88921001926782195</v>
+      </c>
+      <c r="C7">
+        <v>0.90366088631984498</v>
+      </c>
+      <c r="D7">
+        <v>0.90944123314065495</v>
+      </c>
+      <c r="E7">
+        <v>0.90173410404624199</v>
+      </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>4</v>
       </c>
+      <c r="B8">
+        <v>0.74497723815453398</v>
+      </c>
+      <c r="C8">
+        <v>0.72920051448630896</v>
+      </c>
+      <c r="D8">
+        <v>0.75937273038006603</v>
+      </c>
+      <c r="E8">
+        <v>0.75096044959988595</v>
+      </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>5</v>
       </c>
+      <c r="B9">
+        <v>0.33965416106201701</v>
+      </c>
+      <c r="C9">
+        <v>0.30483835802873099</v>
+      </c>
+      <c r="D9">
+        <v>0.391302207253655</v>
+      </c>
+      <c r="E9">
+        <v>0.24928691132307601</v>
+      </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A10" s="1" t="s">
@@ -5162,16 +5164,52 @@
       <c r="A11" t="s">
         <v>3</v>
       </c>
+      <c r="B11">
+        <v>0.89739884393063496</v>
+      </c>
+      <c r="C11">
+        <v>0.91329479768786104</v>
+      </c>
+      <c r="D11">
+        <v>0.91040462427745605</v>
+      </c>
+      <c r="E11">
+        <v>0.91473988439306297</v>
+      </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>4</v>
       </c>
+      <c r="B12">
+        <v>0.74659429699980195</v>
+      </c>
+      <c r="C12">
+        <v>0.70275058885701103</v>
+      </c>
+      <c r="D12">
+        <v>0.68753068299613396</v>
+      </c>
+      <c r="E12">
+        <v>0.69029885923968404</v>
+      </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>5</v>
       </c>
+      <c r="B13">
+        <v>0.312607600362107</v>
+      </c>
+      <c r="C13">
+        <v>0.29214170134036299</v>
+      </c>
+      <c r="D13">
+        <v>0.35768939425415203</v>
+      </c>
+      <c r="E13">
+        <v>0.24528983152735701</v>
+      </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A14" s="1" t="s">
@@ -5182,15 +5220,51 @@
       <c r="A15" t="s">
         <v>3</v>
       </c>
+      <c r="B15" t="s">
+        <v>12</v>
+      </c>
+      <c r="C15" t="s">
+        <v>12</v>
+      </c>
+      <c r="D15">
+        <v>0.89017341040462405</v>
+      </c>
+      <c r="E15">
+        <v>0.89161849710982599</v>
+      </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B16" t="s">
+        <v>12</v>
+      </c>
+      <c r="C16" t="s">
+        <v>12</v>
+      </c>
+      <c r="D16">
+        <v>0.57842307051019703</v>
+      </c>
+      <c r="E16">
+        <v>0.71437121686976501</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>5</v>
+      </c>
+      <c r="B17" t="s">
+        <v>12</v>
+      </c>
+      <c r="C17" t="s">
+        <v>12</v>
+      </c>
+      <c r="D17">
+        <v>0.470910762254172</v>
+      </c>
+      <c r="E17">
+        <v>0.297191883975158</v>
       </c>
     </row>
   </sheetData>
@@ -5218,6 +5292,54 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
+  <conditionalFormatting sqref="B15:C15">
+    <cfRule type="colorScale" priority="17">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B15:C15">
+    <cfRule type="colorScale" priority="16">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B16:C16">
+    <cfRule type="colorScale" priority="15">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B16:C16">
+    <cfRule type="colorScale" priority="14">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
   <conditionalFormatting sqref="B3:C3">
     <cfRule type="colorScale" priority="35">
       <colorScale>
@@ -5460,54 +5582,6 @@
   </conditionalFormatting>
   <conditionalFormatting sqref="B8:E8">
     <cfRule type="colorScale" priority="25">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B15:C15">
-    <cfRule type="colorScale" priority="17">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B15:C15">
-    <cfRule type="colorScale" priority="16">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B16:C16">
-    <cfRule type="colorScale" priority="15">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B16:C16">
-    <cfRule type="colorScale" priority="14">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>

</xml_diff>